<commit_message>
chore: foodDB 간식 컬럼 삭제
</commit_message>
<xml_diff>
--- a/src/lib/assets/data/fooddb.xlsx
+++ b/src/lib/assets/data/fooddb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkjju/Desktop/nuseum-production/nuseum/src/lib/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1C7838-2303-E947-82F9-63E83EA58F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA73C5A-198C-9342-883B-72C42997D022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1320" windowWidth="27900" windowHeight="16680" xr2:uid="{C9B2B1D6-6CFF-EB43-9CED-D1403F065A2C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="144">
   <si>
     <t>채소</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -536,10 +536,6 @@
   </si>
   <si>
     <t>임페리얼분유 XO Royal Class 1</t>
-  </si>
-  <si>
-    <t>간식</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>목이버섯</t>
@@ -1102,7 +1098,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1138,9 +1134,7 @@
       <c r="J1" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>127</v>
-      </c>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
@@ -1339,19 +1333,19 @@
         <v>56</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>57</v>
@@ -1371,17 +1365,17 @@
         <v>59</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>60</v>
@@ -1401,32 +1395,32 @@
         <v>62</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>63</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>100</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1434,32 +1428,32 @@
         <v>64</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>101</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1467,32 +1461,32 @@
         <v>66</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>67</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>102</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1500,32 +1494,32 @@
         <v>68</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>69</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>103</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1533,32 +1527,32 @@
         <v>70</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>104</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1566,32 +1560,32 @@
         <v>72</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>73</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>105</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1599,32 +1593,32 @@
         <v>74</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>75</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>106</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1632,772 +1626,772 @@
         <v>76</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>77</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>107</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>78</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>108</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>109</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>80</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>110</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>81</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>111</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>112</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>113</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>114</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J25" s="11" t="s">
         <v>115</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>116</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>117</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J28" s="11" t="s">
         <v>118</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>119</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>120</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>121</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>122</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>123</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>124</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>121</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>122</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J37" s="11" t="s">
         <v>123</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>124</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J39" s="11" t="s">
         <v>125</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>126</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2419,31 +2413,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19" thickBot="1">
       <c r="A1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2492,7 +2486,7 @@
         <v>61</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>23</v>
@@ -2570,7 +2564,7 @@
         <v>59</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>16</v>
@@ -2654,7 +2648,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>57</v>
@@ -2702,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2717,7 +2711,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>42</v>
@@ -2735,7 +2729,7 @@
     <row r="12" spans="1:9">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="5" t="s">
@@ -2782,7 +2776,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="2"/>
       <c r="I14" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2799,7 +2793,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2816,7 +2810,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2870,7 +2864,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:6">

</xml_diff>